<commit_message>
fluxo certo agora vamos ajeitar o fluxo
</commit_message>
<xml_diff>
--- a/resumos.xlsx
+++ b/resumos.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -465,111 +465,130 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.finep.gov.br/chamadas-publicas/chamadapublica/764</t>
+          <t>https://sebrae.com.br/sites/PortalSebrae/parceirodomunicipio/cidadeempreendedora/inovacao-e-sustentabilidade,88faf8298baaf810VgnVCM1000001b00320aRCRD</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>CHAMADA PÚBLICA MCTI/FINEP/FNDCT INFRAESTRUTURA PARA A AMAZÔNIA LEGAL - PRÓ-AMAZÔNIA 2025 SELEÇÃO PÚBLICA DE PROPOSTAS PARA O APOIO FINANCEIRO VISANDO O DESENVOLVIMENTO DE INFRAESTRUTURA DE PESQUISA CIENTÍFICA E TECNOLÓGICA NA REGIÃO DA AMAZÔNIA LEGAL Selecionar propostas para concessão de apoio financeiro à execução de projetos, de ICTs isoladamente ou em Rede, visando a expansão e a interiorização da infraestrutura de pesquisa científica e tecnológica na região da Amazônia Legal. Término do prazo para envio do Cadastro na Plataforma de Apoio e Financiamento da Finep (segmentos "Básico de Pessoa Jurídica" e "Documentos Institucionais") 12/01/2026   O que é esta Chamada Pública?Seleção pública para apoio financeiro a projetos voltados à expansão e interiorização da infraestrutura de pesquisa científica e tecnológica na Amazônia Legal. Os projetos podem ser submetidos: Quem pode participar? Áreas temáticas apoiadas  A proposta deve se enquadrar em uma das seguintes áreas: Limite de submissões: até 3 propostas por Instituição Executora, em rede ou não. O que pode ser financiado?</t>
+          <t>Crie sua Conta Sebrae agora e tenha acesso gratuito a conteúdos e serviços imperdíveis. Já tenho uma conta.Entrar Fortalecendo o desenvolvimento local com soluções criativas e sustentáveis que geram riqueza, preservam o ambiente e melhoram a qualidade de vida  Quando se fala em inovação, muitas vezes associamos o termo às transformações tecnológicas e digitais, como inteligência artificial, robôs, carros autônomos e todas as novidades que vêm invadindo o nosso cotidiano. Mas o processo inovador não precisa da tecnologia para existir; ou melhor, é bem mais amplo do que qualquer ferramenta tecnológica. Inovação significa criar novas formas de fazer algo. É gerar riqueza e crescimento econômico por meio de ideias e soluções criativas.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.finep.gov.br/chamadas-publicas/chamadapublica/762</t>
+          <t>https://esginside.com.br/2025/09/30/tecnologias-limpas-e-transformacao-digital-impulsionam-solucoes-sustentaveis-no-brasil/</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>SELEÇÃO DE FUNDOS DE INVESTIMENTO EM PARTICIPAÇÕES DE BIOECONOMIA E SUSTENTABILIDADE (FIP Bioeconomia e Sustentabilidade) A Financiadora de Estudos e Projetos (“Finep”), na qualidade de secretaria executiva do Fundo Nacional de Desenvolvimento Científico e Tecnológico (“FNDCT”) vem, por intermédio desta Chamada Pública, convidar Administradores de Carteiras de Valores Mobiliários, registrados na categoria “gestor de recursos” (“GESTOR”), assim definido pela Instrução CVM nº 175/2022, a apresentar proposta (“PROPOSTA”) para a subscrição de capital em um fundo de investimento em participações já estruturado até a data de envio desta proposta, conforme as características descritas neste Edital. Em caso de dúvidas e orientações sobre o edital, por gentileza, enviar e-mail para Equipe: cp_fipbioeconomia@finep.gov.br  cp_fipbioeconomia@finep.gov.br   Fale com a Finep   Endereços e telefones da Finep</t>
+          <t>Compartilhar O debate sobre o papel das tecnologias limpas na construção de um futuro sustentável reuniu três especialistas ligados ao IEEE: Teresa Cristina de Carvalho, professora da Escola Politécnica da USP; Otavio Chase, da Universidade Federal Rural da Amazônia (UFRA); e Vanessa Schramm, professora da Universidade Federal de Campina Grande (UFCG). Cada um trouxe perspectivas complementares sobre como ciência e inovação podem reduzir desigualdades, preservar recursos e ampliar o desenvolvimento econômico. Teresa Cristina de Carvalho apresentou projetos que unem preservação da floresta e tecnologia de ponta. Segundo ela, o programa Amazônia 4.0 busca instrumentalizar cadeias de produção sustentáveis com recursos da Indústria 4.0, promovendo rastreabilidade via IoT e QR Code e a distribuição equitativa dos benefícios para comunidades locais. Entre os exemplos, Teresa citou o projeto da cadeia do cacau e do cupuaçu, que utiliza estruturas geodésicas movidas a energia solar no Pará para capacitar indígenas e quilombolas na produção de chocolates de alto valor agregado no meio da flroesta.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.bndes.gov.br/wps/portal/site/home/mercado-de-capitais/fundos-de-investimentos/chamadas-publicas-para-selecao-de-fundos</t>
+          <t>https://www.linkedin.com/pulse/o-papel-da-sustentabilidade-digital-como-inovar-sem-perder-qtisf/</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Renderizado em 1/7/26 9:34 AM A seleção de Fundos será realizada por meio de Chamada Pública realizada pelo Sistema BNDES ou por meio de Consulta Prévia, desde que observados os critérios abaixo. A seleção de fundos e seus gestores pode ser feita por meio da realização de Chamadas Públicas específicas ou multissetoriais. Cada Chamada Pública é precedida de uma avaliação que busca identificar as necessidades e oportunidades de investimentos em determinados setores do mercado, cadeias produtivas ou regiões para, combinada com a análise e planejamento da carteira de valores mobiliários, atender às diretrizes estratégicas do Sistema BNDES. Numa Chamada Pública para seleção de um fundo e seu gestor, são definidos e informados aos participantes da concorrência o objetivo e critérios do processo de seleção, dentre eles: (i) objetivo da Chamada Pública; (ii) participação máxima do Sistema BNDES; (iii) critérios eliminatórios e classificatórios para a seleção dos fundos; e (iv) formas de remuneração. Os interessados em participar do processo seletivo formalizam uma Consulta Prévia com a proposta do fundo e a encaminham ao Sistema BNDES.</t>
+          <t>Agree &amp; Join LinkedIn
+      By clicking Continue to join or sign in, you agree to LinkedIn’s User Agreement, Privacy Policy, and Cookie Policy. Create your free account or sign in to continue your search
+              or
+      By clicking Continue to join or sign in, you agree to LinkedIn’s User Agreement, Privacy Policy, and Cookie Policy. New to LinkedIn? Join now
+                          or
+                    New to LinkedIn? Join now
+      By clicking Continue to join or sign in, you agree to LinkedIn’s User Agreement, Privacy Policy, and Cookie Policy.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.gov.br/mcti/pt-br/acompanhe-o-mcti/noticias/2025/11/mcti-e-finep-lancam-tres-editais-para-pesquisas-em-sustentabilidade-na-cop30</t>
+          <t>https://www.gov.br/secom/pt-br/assuntos/noticias/2026/01/com-foco-em-inovacao-e-sustentabilidade-nova-industria-brasil-acelera-reindustrializacao-do-pais</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Notícias COP30 
-    No total, serão investidos R$ 460 milhões nos editais Foto: Luara Baggi/ASCOM MCTI
-   O Ministério de Ciência, Tecnologia e Inovação (MCTI) e a Financiadora de Estudos e Projetos (Finep), empresa pública vinculada à pasta, lançaram, nesta terça-feira (11), três editais de investimento para empresas e instituições de pesquisas em sustentabilidade. O anúncio ocorreu durante a 30ª Conferência das Nações Unidas sobre Mudanças Climáticas (COP30), que ocorre em Belém (PA), até 21 de novembro. Para a ministra do MCTI, Luciana Santos, o investimento mostra o compromisso do Governo do Brasil com o desenvolvimento sustentável, com a preservação da diversidade e a memória brasileira e com a agenda climática. “Todas essas iniciativas mostram que a ciência brasileira está pronta para liderar soluções na agenda climática, que o Brasil é parte da resposta global aos desafios do nosso tempo e que o desenvolvimento que queremos passa por respeitar e valorizar a cultura, a diversidade, os povos, os nossos saberes e a nossa soberania”, disse. No total, serão investidos R$ 460 milhões.</t>
+          <t>Notícias BALANÇO 2025 
+    O programa Mover é um dos maiores símbolos desse novo momento, com a atração de investimentos e o fortalecimento da cadeia automotiva
+    - Foto:
+    Ricardo Stuckert/PR
+   Ao longo de 2025, o Brasil consolidou a retomada dos investimentos na indústria, na inovação e na geração de empregos. A política da Nova Indústria Brasil (NIB) mostra, na prática, como o dinheiro público bem aplicado se transforma em crescimento econômico, mais oportunidades de trabalho e produtos melhores para a população. Os recursos do Plano Mais Produção, instrumento de financiamento da NIB, saltaram para R$ 643,3 bilhões no último ano. Desse total, já foram destinados R$ 588,4 bilhões, entre 2023 e 2025, para 406 mil projetos em todas as regiões, alinhados às seis missões da NIB. Dinheiro que fortaleceu fábricas, modernizou máquinas, estimulou novas tecnologias e ajudou empresas de todos os tamanhos a produzir mais, com eficiência e sustentabilidade.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://agenciadenoticias.bndes.gov.br/bndes/Edital-do-BNDES-para-selecionar-fundos-em-economia-verde-vai-movimentar-R%24-18-bi-em-investimentos/</t>
+          <t>https://mittechreview.com.br/transformacao-digital-sustentavel-rumo-a-um-mundo-mais-responsavel-e-inovador/</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>O Banco Nacional de Desenvolvimento Econômico e Social (BNDES) lança, nesta segunda-feira, 1º de setembro, a Chamada de Clima, edital público com orçamento de até R$ 5 bilhões para selecionar fundos de investimento estruturados para projetos de descarbonização de processos industriais, transição energética, infraestrutura para adaptação climática, tecnologia para agricultura verde, restauração ecológica, reflorestamento e conservação de florestas. A Chamada de Clima integra a estratégia de retomada de investimentos da BNDES Participações S.A. (BNDESPAR), subsidiária integral do BNDES, em renda variável e prevê investimentos em dois tipos de fundos (já existentes ou que sejam criados para esse fim): Fundos de Equity e Fundos de Crédito. As propostas poderão ser cadastradas até o dia 20 de outubro deste ano e podem incluir investidores estrangeiros. O resultado será divulgado em janeiro de 2026. Serão selecionados até cinco de fundos de equity, totalizando até R$ 4 bilhões em aporte do BNDES, sendo até três na Modalidade de Apoio de Transformação Ecológica (transição energética, ecológica, tecnologia para agricultura verde e descarbonização) e até dois na Modalidade de Apoio de Soluções Baseadas na Natureza (reflorestamento, agroflorestas, manejo florestal sustentável, silvicultura regenerativa, preservação e recuperação de ecossistemas e biodiversidade).</t>
+          <t>A Transformação Digital é uma oportunidade para empresas integrarem sustentabilidade em suas operações, promovendo um futuro responsável e competitivo. A combinação disso com tecnologias avançadas permite enfrentar desafios globais e prosperar em um mundo em evolução. A Transformação Digital não é apenas uma revolução tecnológica, mas também uma oportunidade crucial para as empresas alinharem suas operações e estratégias com a sustentabilidade, promovendo um futuro mais responsável e competitivo. A convergência desses dois conceitos não apenas impulsiona a eficiência, mas também abre portas para a inovação, a transparência e a responsabilidade, gerando diferenciais competitivos significativos. Sabemos que a TD permite que as empresas otimizem suas operações de maneira mais eficiente, podendo ser, ademais, sustentável.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://swissnex.org/brazil/discover/open-calls/</t>
+          <t>https://jornaldaindustria.com.br/tecnologia/rota-da-inovacao-aposta-em-solucoes-sustentaveis-e-digitais-para-transformar-o-brasil</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Check out open calls of Swissnex in Brazil, the Swissnex Network, and our partners. Call for Applications for a journey where artistic imagination meets scientific knowledge, from the Amazonia to Rome; deadline 30 January 2026. Are you a Swiss startup ready to connect with the Brazilian market? Access Brazil. Validate your market.</t>
+          <t>A jornada de inovação que percorrerá o Brasil em busca de tecnologias para transição ecológica e digital representa uma iniciativa estratégica que visa acelerar o desenvolvimento sustentável do país. A ação, coordenada pela Mobilização Empresarial pela Inovação (MEI), do Sistema Indústria, pretende mapear e conectar soluções inovadoras que possam impulsionar a transformação verde e digital em diversos setores produtivos. O projeto começa em julho e promete envolver ecossistemas de inovação regionais com foco em resultados práticos. A jornada de inovação que percorrerá o Brasil em busca de tecnologias para transição ecológica e digital passará por 14 estados, com eventos, visitas técnicas e encontros com startups, universidades, centros de pesquisa e empresas. A ideia é formar uma ponte entre os desafios industriais e as soluções tecnológicas capazes de oferecer mais eficiência, sustentabilidade e competitividade às empresas brasileiras.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.brde.com.br/fundo-verde/</t>
+          <t>https://www.bv.com.br/bv-inspira/sustentabilidade/inovacao-e-sustentabilidade</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>você está em: INSTITUCIONAL O BANCO VERDE BRDE é um conjunto de iniciativas para a promoção de impacto socioambiental e climático positivo na Região Sul do Brasil. Contempla três eixos de ação: O FUNDO VERDE E DE EQUIDADE é um fundo de natureza operacional e financeira constituído para atuação específica do BANCO VERDE BRDE em seu EIXO II mediante apoio financeiro a projetos socioambientais e climáticos, nas seguintes categorias: Edital CAMP VIVA ÁGUA – Impactos Positivos para a segurança hídrica – Inscrições abertas  Estão abertas as inscrições para a Teia de Soluções | CAMP Viva Água – Impactos positivos para a segurança hídrica, processo que vai selecionar, capacitar e apoiar financeiramente projetos ambientais em territórios estratégicos de cinco estados brasileiros. No Paraná, a iniciativa tem participação direta do Banco Regional de Desenvolvimento do Extremo Sul (BRDE), parceiro institucional da Fundação Grupo Boticário na realização do projeto. Inscrições: até 13 de fevereiro de 2026, às 18h Informações e edital: https://camp.teiadesolucoes.com.br/Inscricoes  O Banco Regional de Desenvolvimento do Extremo Sul (BRDE) torna pública a presente chamada para seleção de projeto de estudos técnicos especializados, com o objetivo de elaborar um Diagnóstico detalhado sobre a situação do saneamento básico em Santa Catarina. Objetivo da Chamada
-Selecionar Plano de Trabalho que contemple diagnóstico técnico sobre abastecimento de água potável, esgotamento sanitário e drenagem urbana, nos termos das diretrizes técnicas previstas no Edital e seus anexos.</t>
+          <t>Descubra mais conteúdos  ESG Publicado em por Equipe BV Inspira Uma pesquisa feita pela Câmara Americana de Comércio (Amcham Brasil) – e divulgada pela CNN Brasil, mostrou que o percentual de companhias onde já são implementadas iniciativas de sustentabilidade passou de 71% para 76%. Esse é um avanço muito relevante e mostra como o tema vem ganhando espaço no mundo corporativo. O próximo passo é ampliar esse movimento, unindo inovação às práticas verdes para gerar cada vez mais valor de forma contínua. Mais do que nunca, existe a oportunidade de criar soluções que tragam retorno financeiro, social e ambiental de forma integrada, fortalecendo tanto os negócios quanto a sociedade. Neste artigo, você vai descobrir o que é inovação e sustentabilidade, por que elas se complementam, quais são os pilares da inovação sustentável e como colocar tudo isso em prática dentro da sua operação para uma gestão eficiente.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.fundobrasil.org.br/edital/geral-2026-fortalecendo-direitos-e-gestando-um-mundo-novo/</t>
+          <t>https://blog.mdftechnology.com.br/ideias-10/</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Conheça a nossa missão, o nosso impacto e a equipe Encontre as vagas em aberto para trabalhar no Fundo Brasil Fortalecemos a sociedade civil organizada brasileira para a promoção e a defesa dos direitos humanos Confira os editais gerais e temáticos Fundos de resposta rápida Apoios diretos para iniciativas estratégicas Para diálogo e aprendizado Acompanhamento individual a projetos Covid-19, Programa Rio Doce e outros Filantropia colaborativa Pesquise a lista completa ou por tema de interesse Notícias, campanhas, blogs, concurso e públicações Nossos apoiadores e como doar PRA TODOS VEREM: Imagem artística em tons de bege. Na esquerda, uma fotografia (tirada de cima) de pessoas em uma audiência, com o crédito da fotógrafa Izabela Chaves – Acervo Fundo Brasil. Logo abaixo, um retrato de Rose Marie Muraro com seu nome e a informação de que essa arte é uma homenagem. Na parte central-direita da imagem o nome “Edital Geral 2026 Fortalecendo direitos e gestando um mundo novo”. No canto inferior direito o logo do Fundo Brasil e a frase “Direitos Humanos.</t>
+          <t>Você já pensou em como as ideias inovadoras podem transformar nosso mundo? A tecnologia desempenha um papel vital na promoção da sustentabilidade, ajudando a criar soluções que beneficiam tanto o meio ambiente quanto a sociedade. Neste post, vamos discutir como as ideias mais brilhantes estão redefinindo o que significa viver de forma sustentável e como cada um de nós pode contribuir para essa mudança positiva. Sumário A tecnologia verde é uma área em crescimento que busca soluções que sejam ao mesmo tempo inovadoras e sustentáveis. Ao integrar princípios ecológicos em processos tecnológicos, podemos desenvolver soluções que limitam o impacto ambiental e promovem práticas de consumo responsáveis.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.gov.br/mdh/pt-br/navegue-por-temas/cooperacao-internacional/editais-2026</t>
+          <t>https://blog.aevo.com.br/inovacao-em-sustentabilidade/</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>&gt; Acesse o modelo de currículo para inscrição nos editais de cooperação técnica internacional e confira os critérios para participação no processo seletivo e para cumprimento de regras da consultoria. Editais abertos Projeto PNUD BRA/18/008 Edital nº 06/2025 - Contratação de consultoria de pessoa física, na modalidade produto, especializada em análise de microdados para realizar a análise detalhada da situação sociodemográficas da população com deficiência no Brasil, visando à formulação de políticas públicas mais eficazes e direcionadas, promovendo a inclusão e a autonomia das pessoas com deficiência no país. INSCRIÇÕES: As pessoas interessadas em participar do processo seletivo deverão encaminhar currículo, conforme modelo disponível em https://www.gov.br/mdh/pt-br/navegue-por-temas/cooperacao-internacional/editais-2025/2025_CV_padrao.docx, para o endereço eletrônico editais.sndpd@mdh.gov.br, a partir do dia 05/12/2025 até 23h59 (horário de Brasília) do dia 20/12/2025. PRORROGAÇÃO: Inscrições prorrogadas do dia 02/01/2026 até 23h59 (horário de Brasília) do dia 06/01/2026. O currículo deverá ser apresentado em formato PDF e obrigatoriamente em língua portuguesa.</t>
+          <t>A inovação em sustentabilidade abrange uma variedade de abordagens e práticas destinadas a criar soluções que atendam às necessidades do presente sem comprometer as gerações futuras. Ao integrar os princípios da sustentabilidade em todas as áreas da economia, a inovação nesse campo visa o equilíbrio entre os aspectos financeiros, sociais e ambientais do desenvolvimento. Nos últimos anos, a inovação em sustentabilidade assumiu um ritmo mais acelarado. Uma prova disso é o aumento considerável no número de patentes relacionadas aos Objetivos de Desenvolvimento Sustentável (ODS). Entre 2005 e 2020, os registros anuais saltaram de aproximadamente 1,8 milhão para mais de 5 milhões.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://centev.ufv.br/sustentabilidade-e-inovacao-caminhos-para-um-futuro-verde/</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Início » Sustentabilidade e Inovação: Caminhos para um Futuro Verde A sustentabilidade é um dos desafios mais urgentes do nosso tempo. Com a crescente preocupação com as mudanças climáticas, a escassez de recursos naturais e a degradação ambiental, a busca por soluções inovadoras se tornou essencial. Startups tecnológicas estão na vanguarda desta transformação, desenvolvendo produtos e serviços que não só atendem às necessidades do presente, mas também preservam o futuro. O papel das startups tecnológicas na promoção da sustentabilidade é crucial. Essas empresas estão utilizando a inovação para criar soluções que abordam problemas ambientais de maneiras novas e eficazes.</t>
         </is>
       </c>
     </row>

</xml_diff>